<commit_message>
New Ipc Distribution File
</commit_message>
<xml_diff>
--- a/Civilworks cost/IPC Distribution.xlsx
+++ b/Civilworks cost/IPC Distribution.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="GoB" sheetId="3" r:id="rId2"/>
     <sheet name="RPA" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="IPC_Dist" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GoB!$A$1:$T$16</definedName>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>O&amp;M During Construction</t>
   </si>
@@ -257,6 +259,45 @@
   </si>
   <si>
     <t>158/KISH-13 6th RA BILL</t>
+  </si>
+  <si>
+    <t>Reg_Rehab_Rehab</t>
+  </si>
+  <si>
+    <t>Reg_CW_Box</t>
+  </si>
+  <si>
+    <t>Khal_Riv_New</t>
+  </si>
+  <si>
+    <t>Khal_Riv_Rehab</t>
+  </si>
+  <si>
+    <t>Full_Emb_Rehab</t>
+  </si>
+  <si>
+    <t>Sub_Emb_Rehab</t>
+  </si>
+  <si>
+    <t>Sub_Emb_Const</t>
+  </si>
+  <si>
+    <t>Reg_Rehab_New</t>
+  </si>
+  <si>
+    <t>Wmg_Office</t>
+  </si>
+  <si>
+    <t>IPCNo</t>
+  </si>
+  <si>
+    <t>156/SUNM-01 4th RA Bill</t>
+  </si>
+  <si>
+    <t>Gob</t>
+  </si>
+  <si>
+    <t>Rpa</t>
   </si>
 </sst>
 </file>
@@ -331,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,6 +426,15 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="M1" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView view="pageBreakPreview" topLeftCell="M4" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView topLeftCell="M55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="M13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
@@ -2589,4 +2639,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2">
+        <v>10121557.060000001</v>
+      </c>
+      <c r="I2">
+        <v>9416806.852</v>
+      </c>
+      <c r="M2">
+        <v>2442296</v>
+      </c>
+      <c r="N2" s="1">
+        <v>17096068</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Civil works cost 1-39
</commit_message>
<xml_diff>
--- a/Civilworks cost/IPC Distribution.xlsx
+++ b/Civilworks cost/IPC Distribution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="109">
   <si>
     <t>O&amp;M During Construction</t>
   </si>
@@ -298,6 +298,63 @@
   </si>
   <si>
     <t>Rpa</t>
+  </si>
+  <si>
+    <t>160/(SUNM-01)-05 2nd RA Bill</t>
+  </si>
+  <si>
+    <t>161/Habi-1 5th  RA Bill</t>
+  </si>
+  <si>
+    <t>172/Kish-12 7th  RA Bill</t>
+  </si>
+  <si>
+    <t>161/Kish-16 9th  RA Bill</t>
+  </si>
+  <si>
+    <t>175/Kish-23 2nd  RA Bill</t>
+  </si>
+  <si>
+    <t>174/Netr-01  4th  RA Bill</t>
+  </si>
+  <si>
+    <t>190/Kish-22 2nd  RA Bill</t>
+  </si>
+  <si>
+    <t>191/Kish-26 6th  RA Bill</t>
+  </si>
+  <si>
+    <t>194/(SUNM-01)-06 6th RA Bill</t>
+  </si>
+  <si>
+    <t>192/(SUNM-01)-04 4th RA Bill</t>
+  </si>
+  <si>
+    <t>195/Netr-06 5th RA Bill</t>
+  </si>
+  <si>
+    <t>193/Kish-05 5th  RA Bill</t>
+  </si>
+  <si>
+    <t>199/Kish-17 10th  RA Bill</t>
+  </si>
+  <si>
+    <t>210/(SUNM-01)-06 6th RA final Bill</t>
+  </si>
+  <si>
+    <t>209/(SUNM-01)-05 2nd RA Bill</t>
+  </si>
+  <si>
+    <t>213/Kish-23 3rd  RA Bill</t>
+  </si>
+  <si>
+    <t>212/(SUNM-02)-02 3rd RA Bill</t>
+  </si>
+  <si>
+    <t>159/Kish-28/Lot-4 1st  RA Bill</t>
+  </si>
+  <si>
+    <t>173/Netr-03 4th RA Bill</t>
   </si>
 </sst>
 </file>
@@ -372,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,6 +492,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2643,22 +2716,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
       <c r="B1" s="24" t="s">
@@ -2702,21 +2784,436 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D2">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="28">
         <v>10121557.060000001</v>
       </c>
-      <c r="I2">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="27">
         <v>9416806.852</v>
       </c>
-      <c r="M2">
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="27">
         <v>2442296</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="27">
         <v>17096068</v>
       </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="27">
+        <v>4153902.9180000001</v>
+      </c>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27">
+        <v>519238</v>
+      </c>
+      <c r="N3" s="27">
+        <v>3634665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="27">
+        <v>31435052</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28">
+        <v>3929382</v>
+      </c>
+      <c r="N4" s="28">
+        <v>27505670</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28">
+        <v>7440653</v>
+      </c>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28">
+        <v>930087</v>
+      </c>
+      <c r="N5" s="28">
+        <v>6510571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28">
+        <v>8773225</v>
+      </c>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28">
+        <v>1096659</v>
+      </c>
+      <c r="N6" s="28">
+        <v>7676616</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="28">
+        <v>967157.26999999955</v>
+      </c>
+      <c r="E7" s="28">
+        <v>7576934.0999999996</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28">
+        <v>1068011</v>
+      </c>
+      <c r="N7" s="28">
+        <v>7476080</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="28">
+        <v>15300148.25</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28">
+        <v>5002242.9400000004</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28">
+        <v>2537799</v>
+      </c>
+      <c r="N8" s="28">
+        <v>17764592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28">
+        <v>6272429.75</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28">
+        <v>784054</v>
+      </c>
+      <c r="N9" s="28">
+        <v>5488375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="28">
+        <v>2376584.4930000007</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28">
+        <v>5851260.3669999996</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28">
+        <v>1028481</v>
+      </c>
+      <c r="N10" s="28">
+        <v>7199364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="28">
+        <v>3951018.61</v>
+      </c>
+      <c r="E11" s="28">
+        <v>1303448.1200000001</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28">
+        <v>3401350.1</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="28">
+        <v>1081977</v>
+      </c>
+      <c r="N11" s="28">
+        <v>7573840</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2725,12 +3222,49 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="G2:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>2913738.14</v>
+      </c>
+    </row>
+    <row r="3" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>2230920.327</v>
+      </c>
+    </row>
+    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>589267.10400000005</v>
+      </c>
+    </row>
+    <row r="5" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>46933.917999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>70400.877999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>SUM(G2:G6)</f>
+        <v>5851260.3669999996</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated IPC Distribution 7
</commit_message>
<xml_diff>
--- a/Civilworks cost/IPC Distribution.xlsx
+++ b/Civilworks cost/IPC Distribution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1354,14 +1354,14 @@
       <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="97.5703125" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="97.5546875" customWidth="1"/>
+    <col min="4" max="4" width="52.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>57</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>4111306_Construction of Irrigation Inlet (New Haors)</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>58</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>4111307_ Re-installation/Construction of Regulator/ Causeway (Rehabilitation Sub-Projects)</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>59</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>4111307_ Installation/Construction of New Regulators/ Causeway/Bridge/Box Drainage Outlet) (New Haors)</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v xml:space="preserve">4111307_ Re-excavation of Khal/River (New Haors) </v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>61</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v xml:space="preserve">4111201_ Re-excavation of Khal/River (Rehabilitation Sub-Projects) </v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>62</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>4111201_ Rehabilitation of Full Embankment (Resection/ construction) (Rehabilitation Sub-Projects)</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>63</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>4111201_ Rehabilitation of Submergible Embankment  (Resection/construction)  (Rehabilitation Sub-Projects)</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>64</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>4111201_Construction of Submersible Embankment (New Haors) (Earth Volume: 29.98 lakh cum)</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>65</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>4111201_ Rehabilitation of Regulator (New Haors)</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>66</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>4111201_Construction of WMG Office</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>67</v>
       </c>
@@ -1553,28 +1553,28 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="115.85546875" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="115.88671875" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="47.109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="44.44140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="56" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="50" customWidth="1"/>
-    <col min="10" max="10" width="61.28515625" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" customWidth="1"/>
-    <col min="12" max="12" width="51.5703125" customWidth="1"/>
-    <col min="13" max="13" width="49.42578125" customWidth="1"/>
-    <col min="14" max="14" width="45.28515625" customWidth="1"/>
-    <col min="15" max="15" width="56.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="42.42578125" customWidth="1"/>
-    <col min="17" max="17" width="43.28515625" customWidth="1"/>
+    <col min="10" max="10" width="61.33203125" customWidth="1"/>
+    <col min="11" max="11" width="43.6640625" customWidth="1"/>
+    <col min="12" max="12" width="51.5546875" customWidth="1"/>
+    <col min="13" max="13" width="49.44140625" customWidth="1"/>
+    <col min="14" max="14" width="45.33203125" customWidth="1"/>
+    <col min="15" max="15" width="56.44140625" style="12" customWidth="1"/>
+    <col min="16" max="16" width="42.44140625" customWidth="1"/>
+    <col min="17" max="17" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>29</v>
@@ -1625,7 +1625,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
     </row>
-    <row r="3" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1671,7 +1671,7 @@
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
     </row>
-    <row r="4" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1712,7 +1712,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
     </row>
-    <row r="5" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
     </row>
-    <row r="6" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1766,7 +1766,7 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
     </row>
-    <row r="7" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1787,7 +1787,7 @@
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
     </row>
-    <row r="8" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
     </row>
-    <row r="9" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>391128</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
     </row>
-    <row r="11" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1883,7 +1883,7 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
     </row>
-    <row r="13" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -1943,23 +1943,23 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="119" customWidth="1"/>
     <col min="2" max="2" width="39" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="8" width="39" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="47.140625" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="47.109375" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="47.5546875" customWidth="1"/>
     <col min="12" max="12" width="52" style="12" customWidth="1"/>
-    <col min="13" max="13" width="48.28515625" customWidth="1"/>
-    <col min="14" max="14" width="48.140625" customWidth="1"/>
-    <col min="15" max="15" width="60.28515625" customWidth="1"/>
-    <col min="16" max="16" width="45.7109375" customWidth="1"/>
-    <col min="17" max="17" width="46.140625" customWidth="1"/>
+    <col min="13" max="13" width="48.33203125" customWidth="1"/>
+    <col min="14" max="14" width="48.109375" customWidth="1"/>
+    <col min="15" max="15" width="60.33203125" customWidth="1"/>
+    <col min="16" max="16" width="45.6640625" customWidth="1"/>
+    <col min="17" max="17" width="46.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>29</v>
@@ -2010,7 +2010,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
     </row>
-    <row r="3" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
     </row>
-    <row r="4" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -2097,7 +2097,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
     </row>
-    <row r="5" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -2128,7 +2128,7 @@
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
     </row>
-    <row r="6" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
     </row>
-    <row r="7" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2172,7 +2172,7 @@
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
     </row>
-    <row r="8" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
     </row>
-    <row r="9" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>2737897</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2247,7 +2247,7 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
     </row>
-    <row r="11" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
     </row>
-    <row r="13" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2328,26 +2328,26 @@
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="16" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="10" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" style="11" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="25.109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" style="10" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="11" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="12">
         <v>7146.0320000000002</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" s="12">
         <v>2175338.3840000001</v>
       </c>
@@ -2389,7 +2389,7 @@
       <c r="O2" s="12"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
         <v>442686.37599999999</v>
       </c>
@@ -2413,7 +2413,7 @@
       <c r="O3" s="12"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" s="12">
         <v>25927.940999999999</v>
       </c>
@@ -2440,7 +2440,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -2475,7 +2475,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="12">
         <v>769684.61699999997</v>
@@ -2500,7 +2500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C7" s="12">
         <v>776580.14399999997</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>12285185.104948564</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C8" s="12">
         <f>SUM(C1:C7)</f>
         <v>2491596.338</v>
@@ -2548,7 +2548,7 @@
         <v>901800.89505143708</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E9" s="12">
         <f>B6+C8</f>
         <v>2491596.338</v>
@@ -2570,12 +2570,12 @@
         <v>15070841</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L12" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L13" s="10" t="s">
         <v>48</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L14" s="16">
         <v>5478066.2400000002</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>4313977.0977821741</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L15" s="16"/>
       <c r="M15" s="12">
         <v>315745.96999999997</v>
@@ -2643,7 +2643,7 @@
         <v>5197670.9022178268</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K16" t="s">
         <v>25</v>
       </c>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="S16" s="10"/>
     </row>
-    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K17" t="s">
         <v>49</v>
       </c>
@@ -2679,18 +2679,18 @@
         <v>12078283.359999999</v>
       </c>
     </row>
-    <row r="18" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:19" x14ac:dyDescent="0.3">
       <c r="L18" s="10"/>
     </row>
-    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:19" x14ac:dyDescent="0.3">
       <c r="L19" s="10"/>
     </row>
-    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:19" x14ac:dyDescent="0.3">
       <c r="L20" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:19" x14ac:dyDescent="0.3">
       <c r="L21" s="10" t="s">
         <v>48</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="11:19" x14ac:dyDescent="0.3">
       <c r="L22" s="10">
         <v>5478066.2400000002</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>479330.43588387553</v>
       </c>
     </row>
-    <row r="23" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:19" x14ac:dyDescent="0.3">
       <c r="L23" s="10"/>
       <c r="M23" s="10">
         <v>315745.96999999997</v>
@@ -2755,7 +2755,7 @@
         <v>577518.56411612465</v>
       </c>
     </row>
-    <row r="24" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
         <v>25</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1207828.0000000002</v>
       </c>
     </row>
-    <row r="25" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>49</v>
       </c>
@@ -2789,12 +2789,12 @@
         <v>12078283.359999999</v>
       </c>
     </row>
-    <row r="35" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N36" t="s">
         <v>48</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>5923319.2699999996</v>
       </c>
     </row>
-    <row r="37" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N37" t="s">
         <v>54</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>317931.49</v>
       </c>
     </row>
-    <row r="38" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N38" t="s">
         <v>25</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
         <v>55</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>5386258.0510686319</v>
       </c>
     </row>
-    <row r="40" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N40" t="s">
         <v>56</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>6037755.4941627374</v>
       </c>
     </row>
-    <row r="41" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N41" t="s">
         <v>57</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>4823437.4547686297</v>
       </c>
     </row>
-    <row r="42" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N42" t="s">
         <v>58</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>16247450.999999998</v>
       </c>
     </row>
-    <row r="43" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N43" t="s">
         <v>25</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>12585254.568999998</v>
       </c>
     </row>
-    <row r="44" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N44" t="s">
         <v>49</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>18826505.328999996</v>
       </c>
     </row>
-    <row r="48" spans="14:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:21" x14ac:dyDescent="0.3">
       <c r="N48" t="s">
         <v>62</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N49" t="s">
         <v>63</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>4142488.1873903489</v>
       </c>
     </row>
-    <row r="50" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N50" t="s">
         <v>64</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>3815450.8126096507</v>
       </c>
     </row>
-    <row r="51" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="14:20" x14ac:dyDescent="0.3">
       <c r="O51" s="10">
         <f>SUM(O49:O50)</f>
         <v>9094786.5099999998</v>
@@ -3021,7 +3021,7 @@
         <v>9094787</v>
       </c>
     </row>
-    <row r="54" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N54" t="s">
         <v>66</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N55" t="s">
         <v>63</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>4142488.1873903489</v>
       </c>
     </row>
-    <row r="56" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N56" t="s">
         <v>64</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>3815450.8126096507</v>
       </c>
     </row>
-    <row r="57" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P57">
         <v>1</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>9094787</v>
       </c>
     </row>
-    <row r="58" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N58" t="s">
         <v>72</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N59" t="s">
         <v>33</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>4989638.1726636579</v>
       </c>
     </row>
-    <row r="60" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N60" t="s">
         <v>64</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>5464314.8273363421</v>
       </c>
     </row>
-    <row r="61" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N61" t="s">
         <v>73</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>10453953</v>
       </c>
     </row>
-    <row r="62" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N62" t="s">
         <v>64</v>
       </c>
@@ -3174,13 +3174,13 @@
         <v>6244931.3999999994</v>
       </c>
     </row>
-    <row r="63" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="14:20" x14ac:dyDescent="0.3">
       <c r="O63" s="10">
         <f>SUM(O59,O62)</f>
         <v>11947375.18</v>
       </c>
     </row>
-    <row r="65" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N65" t="s">
         <v>75</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N66" t="s">
         <v>59</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>4989638.1726636579</v>
       </c>
     </row>
-    <row r="67" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N67" t="s">
         <v>64</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>5464314.8273363421</v>
       </c>
     </row>
-    <row r="68" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N68" t="s">
         <v>73</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>10453953</v>
       </c>
     </row>
-    <row r="69" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N69" t="s">
         <v>64</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>6244931.3999999994</v>
       </c>
     </row>
-    <row r="70" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="14:20" x14ac:dyDescent="0.3">
       <c r="O70" s="12">
         <v>11947375.18</v>
       </c>
@@ -3277,32 +3277,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="L108" sqref="L108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="49.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="17" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" customWidth="1"/>
+    <col min="16" max="17" width="16.44140625" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" customWidth="1"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>117</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>5</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>6</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>10</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>11</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>12</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>14</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32">
         <v>15</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="29">
         <v>16</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>17</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>18</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="29">
         <v>19</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
         <v>20</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>21</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>22</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>23</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>24</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="29">
         <v>25</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>26</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="29">
         <v>27</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>28</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="29">
         <v>29</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="29">
         <v>30</v>
       </c>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="29">
         <v>31</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>32</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="29">
         <v>33</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="29">
         <v>34</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="32">
         <v>35</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>36</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>37</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>38</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>39</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>40</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>41</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>42</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>44</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>45</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>46</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>47</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>48</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>49</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>50</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>51</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>52</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>53</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>54</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>55</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>56</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>57</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>58</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>59</v>
       </c>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="S60" s="10"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>60</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>61</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>62</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>63</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>64</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>65</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
         <v>66</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <v>67</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>68</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
         <v>69</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="29">
         <v>70</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <v>71</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="29">
         <v>72</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="29">
         <v>73</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>74</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>75</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="29">
         <v>76</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="29">
         <v>77</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="29">
         <v>78</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="29">
         <v>79</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="29">
         <v>80</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="29">
         <v>81</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <v>82</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="29">
         <v>83</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="29">
         <v>84</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="29">
         <v>85</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="29">
         <v>86</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="29">
         <v>87</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="29">
         <v>88</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <v>89</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="29">
         <v>90</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="29">
         <v>91</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="29">
         <v>92</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="29">
         <v>93</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="29">
         <v>94</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="29">
         <v>95</v>
       </c>
@@ -6680,7 +6680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="29">
         <v>96</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="29">
         <v>97</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="29">
         <v>98</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="29">
         <v>99</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="29">
         <v>100</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="29">
         <v>101</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="29">
         <v>102</v>
       </c>
@@ -6942,21 +6942,21 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G2" s="1" t="s">
         <v>63</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G3" s="1">
         <v>17644936.100000001</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>204301.34</v>
       </c>
     </row>
-    <row r="4" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G4" s="1">
         <v>-166123.07999999999</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>98414.79</v>
       </c>
     </row>
-    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G5" s="1">
         <v>4900152.0999999996</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>3557905.85</v>
       </c>
     </row>
-    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G6" s="1">
         <v>286245</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>866744.93</v>
       </c>
     </row>
-    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G7" s="1">
         <v>619378.32999999996</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>161285.35999999999</v>
       </c>
     </row>
-    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G8" s="12">
         <f>SUM(G3:G7)</f>
         <v>23284588.450000003</v>
@@ -7013,7 +7013,7 @@
         <v>15775.98</v>
       </c>
     </row>
-    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G9" s="12">
         <v>28737182.920000002</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>14288.02</v>
       </c>
     </row>
-    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G10" s="12">
         <f>G9-G8</f>
         <v>5452594.4699999988</v>
@@ -7030,13 +7030,13 @@
         <v>53423.24</v>
       </c>
     </row>
-    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:9" x14ac:dyDescent="0.3">
       <c r="I11" s="12">
         <f>SUM(I3:I10)</f>
         <v>4972139.5100000007</v>
       </c>
     </row>
-    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E15" s="1">
         <v>875966.73300000001</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>46900.13</v>
       </c>
     </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E16" s="1">
         <v>906433.66399999999</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>2590080.1800000002</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E17" s="1">
         <f>SUM(E15:E16)</f>
         <v>1782400.3969999999</v>
@@ -7069,7 +7069,7 @@
         <v>1949709.13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E18" s="1">
         <v>7172327.3300000001</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>1366206.83</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E19" s="12">
         <f>E18-E17</f>
         <v>5389926.9330000002</v>
@@ -7086,23 +7086,23 @@
         <v>739134.85</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G20" s="1">
         <v>379009.28000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G21" s="1">
         <v>600581.69999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G22" s="1">
         <f>SUM(G15:G21)</f>
         <v>7671622.0999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>106</v>
       </c>
@@ -7143,16 +7143,16 @@
       <selection activeCell="A2" sqref="A2:N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>104</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>4232587</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>105</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>8992806</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>106</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>5502837.0250000004</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>107</v>
       </c>
@@ -7260,7 +7260,7 @@
         <v>3191592</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>108</v>
       </c>
@@ -7286,7 +7286,7 @@
         <v>6275786</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>109</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>3061893</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>110</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>18223550</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>111</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>3211140</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>112</v>
       </c>

</xml_diff>

<commit_message>
DPP Old New Comparision
</commit_message>
<xml_diff>
--- a/Civilworks cost/IPC Distribution.xlsx
+++ b/Civilworks cost/IPC Distribution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="-60" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
     <sheet name="Package_wise_cost" sheetId="9" r:id="rId6"/>
+    <sheet name="Monthly_Rpa" sheetId="11" r:id="rId7"/>
+    <sheet name="Monthly_Gob" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="316">
   <si>
     <t>O&amp;M During Construction</t>
   </si>
@@ -933,6 +935,45 @@
   </si>
   <si>
     <t>KISH-28/Lot-3</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1094,12 +1135,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFF99"/>
+      <color rgb="FF336699"/>
+      <color rgb="FF6699FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1380,14 +1439,14 @@
       <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="97.5546875" customWidth="1"/>
-    <col min="4" max="4" width="52.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="97.5703125" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1398,7 +1457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>57</v>
       </c>
@@ -1413,7 +1472,7 @@
         <v>4111306_Construction of Irrigation Inlet (New Haors)</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>58</v>
       </c>
@@ -1428,7 +1487,7 @@
         <v>4111307_ Re-installation/Construction of Regulator/ Causeway (Rehabilitation Sub-Projects)</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>59</v>
       </c>
@@ -1443,7 +1502,7 @@
         <v>4111307_ Installation/Construction of New Regulators/ Causeway/Bridge/Box Drainage Outlet) (New Haors)</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -1458,7 +1517,7 @@
         <v xml:space="preserve">4111307_ Re-excavation of Khal/River (New Haors) </v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>61</v>
       </c>
@@ -1473,7 +1532,7 @@
         <v xml:space="preserve">4111201_ Re-excavation of Khal/River (Rehabilitation Sub-Projects) </v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>62</v>
       </c>
@@ -1488,7 +1547,7 @@
         <v>4111201_ Rehabilitation of Full Embankment (Resection/ construction) (Rehabilitation Sub-Projects)</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>63</v>
       </c>
@@ -1503,7 +1562,7 @@
         <v>4111201_ Rehabilitation of Submergible Embankment  (Resection/construction)  (Rehabilitation Sub-Projects)</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>64</v>
       </c>
@@ -1518,7 +1577,7 @@
         <v>4111201_Construction of Submersible Embankment (New Haors) (Earth Volume: 29.98 lakh cum)</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>65</v>
       </c>
@@ -1533,7 +1592,7 @@
         <v>4111201_ Rehabilitation of Regulator (New Haors)</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>66</v>
       </c>
@@ -1548,7 +1607,7 @@
         <v>4111201_Construction of WMG Office</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>67</v>
       </c>
@@ -1575,30 +1634,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="M27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="22.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" customWidth="1"/>
-    <col min="13" max="13" width="25.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="26.33203125" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="14.88671875" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" customWidth="1"/>
-    <col min="21" max="21" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="5">
         <v>7146.0320000000002</v>
       </c>
@@ -1614,7 +1673,7 @@
       <c r="O1" s="5"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="5">
         <v>2175338.3840000001</v>
       </c>
@@ -1640,7 +1699,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>442686.37599999999</v>
       </c>
@@ -1664,7 +1723,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>25927.940999999999</v>
       </c>
@@ -1691,7 +1750,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1726,7 +1785,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5">
         <v>769684.61699999997</v>
@@ -1751,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="5">
         <v>776580.14399999997</v>
       </c>
@@ -1775,7 +1834,7 @@
         <v>12285185.104948564</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <f>SUM(C1:C7)</f>
         <v>2491596.338</v>
@@ -1799,7 +1858,7 @@
         <v>901800.89505143708</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E9" s="5">
         <f>B6+C8</f>
         <v>2491596.338</v>
@@ -1821,12 +1880,12 @@
         <v>15070841</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1843,7 +1902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L14" s="8">
         <v>5478066.2400000002</v>
       </c>
@@ -1869,7 +1928,7 @@
         <v>4313977.0977821741</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L15" s="8"/>
       <c r="M15" s="5">
         <v>315745.96999999997</v>
@@ -1894,7 +1953,7 @@
         <v>5197670.9022178268</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
         <v>14</v>
       </c>
@@ -1920,7 +1979,7 @@
       </c>
       <c r="S16" s="3"/>
     </row>
-    <row r="17" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
         <v>30</v>
       </c>
@@ -1930,18 +1989,18 @@
         <v>12078283.359999999</v>
       </c>
     </row>
-    <row r="18" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L21" s="3" t="s">
         <v>29</v>
       </c>
@@ -1958,7 +2017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L22" s="3">
         <v>5478066.2400000002</v>
       </c>
@@ -1983,7 +2042,7 @@
         <v>479330.43588387553</v>
       </c>
     </row>
-    <row r="23" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L23" s="3"/>
       <c r="M23" s="3">
         <v>315745.96999999997</v>
@@ -2006,7 +2065,7 @@
         <v>577518.56411612465</v>
       </c>
     </row>
-    <row r="24" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K24" t="s">
         <v>14</v>
       </c>
@@ -2032,7 +2091,7 @@
         <v>1207828.0000000002</v>
       </c>
     </row>
-    <row r="25" spans="11:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>30</v>
       </c>
@@ -2040,12 +2099,12 @@
         <v>12078283.359999999</v>
       </c>
     </row>
-    <row r="35" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N36" t="s">
         <v>29</v>
       </c>
@@ -2053,7 +2112,7 @@
         <v>5923319.2699999996</v>
       </c>
     </row>
-    <row r="37" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N37" t="s">
         <v>33</v>
       </c>
@@ -2061,7 +2120,7 @@
         <v>317931.49</v>
       </c>
     </row>
-    <row r="38" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
         <v>14</v>
       </c>
@@ -2079,7 +2138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N39" t="s">
         <v>34</v>
       </c>
@@ -2106,7 +2165,7 @@
         <v>5386258.0510686319</v>
       </c>
     </row>
-    <row r="40" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N40" t="s">
         <v>35</v>
       </c>
@@ -2133,7 +2192,7 @@
         <v>6037755.4941627374</v>
       </c>
     </row>
-    <row r="41" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N41" t="s">
         <v>36</v>
       </c>
@@ -2160,7 +2219,7 @@
         <v>4823437.4547686297</v>
       </c>
     </row>
-    <row r="42" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N42" t="s">
         <v>37</v>
       </c>
@@ -2184,7 +2243,7 @@
         <v>16247450.999999998</v>
       </c>
     </row>
-    <row r="43" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
         <v>14</v>
       </c>
@@ -2193,7 +2252,7 @@
         <v>12585254.568999998</v>
       </c>
     </row>
-    <row r="44" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N44" t="s">
         <v>30</v>
       </c>
@@ -2202,7 +2261,7 @@
         <v>18826505.328999996</v>
       </c>
     </row>
-    <row r="48" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N48" t="s">
         <v>41</v>
       </c>
@@ -2210,7 +2269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N49" t="s">
         <v>42</v>
       </c>
@@ -2230,7 +2289,7 @@
         <v>4142488.1873903489</v>
       </c>
     </row>
-    <row r="50" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N50" t="s">
         <v>43</v>
       </c>
@@ -2250,7 +2309,7 @@
         <v>3815450.8126096507</v>
       </c>
     </row>
-    <row r="51" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="14:20" x14ac:dyDescent="0.25">
       <c r="O51" s="3">
         <f>SUM(O49:O50)</f>
         <v>9094786.5099999998</v>
@@ -2272,7 +2331,7 @@
         <v>9094787</v>
       </c>
     </row>
-    <row r="54" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N54" t="s">
         <v>44</v>
       </c>
@@ -2280,7 +2339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N55" t="s">
         <v>42</v>
       </c>
@@ -2297,7 +2356,7 @@
         <v>4142488.1873903489</v>
       </c>
     </row>
-    <row r="56" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N56" t="s">
         <v>43</v>
       </c>
@@ -2314,7 +2373,7 @@
         <v>3815450.8126096507</v>
       </c>
     </row>
-    <row r="57" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="14:20" x14ac:dyDescent="0.25">
       <c r="P57">
         <v>1</v>
       </c>
@@ -2328,7 +2387,7 @@
         <v>9094787</v>
       </c>
     </row>
-    <row r="58" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N58" t="s">
         <v>45</v>
       </c>
@@ -2342,7 +2401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N59" t="s">
         <v>18</v>
       </c>
@@ -2369,7 +2428,7 @@
         <v>4989638.1726636579</v>
       </c>
     </row>
-    <row r="60" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N60" t="s">
         <v>43</v>
       </c>
@@ -2396,7 +2455,7 @@
         <v>5464314.8273363421</v>
       </c>
     </row>
-    <row r="61" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N61" t="s">
         <v>46</v>
       </c>
@@ -2416,7 +2475,7 @@
         <v>10453953</v>
       </c>
     </row>
-    <row r="62" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N62" t="s">
         <v>43</v>
       </c>
@@ -2425,13 +2484,13 @@
         <v>6244931.3999999994</v>
       </c>
     </row>
-    <row r="63" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="14:20" x14ac:dyDescent="0.25">
       <c r="O63" s="3">
         <f>SUM(O59,O62)</f>
         <v>11947375.18</v>
       </c>
     </row>
-    <row r="65" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N65" t="s">
         <v>47</v>
       </c>
@@ -2445,7 +2504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N66" t="s">
         <v>38</v>
       </c>
@@ -2468,7 +2527,7 @@
         <v>4989638.1726636579</v>
       </c>
     </row>
-    <row r="67" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N67" t="s">
         <v>43</v>
       </c>
@@ -2489,7 +2548,7 @@
         <v>5464314.8273363421</v>
       </c>
     </row>
-    <row r="68" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N68" t="s">
         <v>46</v>
       </c>
@@ -2506,7 +2565,7 @@
         <v>10453953</v>
       </c>
     </row>
-    <row r="69" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N69" t="s">
         <v>43</v>
       </c>
@@ -2514,7 +2573,7 @@
         <v>6244931.3999999994</v>
       </c>
     </row>
-    <row r="70" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="14:20" x14ac:dyDescent="0.25">
       <c r="O70" s="5">
         <v>11947375.18</v>
       </c>
@@ -2528,32 +2587,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.44140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" customWidth="1"/>
-    <col min="16" max="17" width="16.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="17" width="16.42578125" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>88</v>
       </c>
@@ -2608,8 +2669,11 @@
       <c r="R1" s="29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2642,8 +2706,11 @@
       <c r="R2" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2676,8 +2743,11 @@
       <c r="R3" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2710,8 +2780,11 @@
       <c r="R4" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2744,8 +2817,11 @@
       <c r="R5" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2778,8 +2854,11 @@
       <c r="R6" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2812,8 +2891,11 @@
       <c r="R7" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2848,8 +2930,11 @@
       <c r="R8" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2882,8 +2967,11 @@
       <c r="R9" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -2918,8 +3006,11 @@
       <c r="R10" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -2954,8 +3045,11 @@
       <c r="R11" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -2990,8 +3084,11 @@
       <c r="R12" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -3028,8 +3125,11 @@
       <c r="R13" s="18">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -3064,8 +3164,11 @@
       <c r="R14" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -3098,8 +3201,11 @@
       <c r="R15" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S15" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>15</v>
       </c>
@@ -3132,8 +3238,11 @@
       <c r="R16" s="20">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S16" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -3168,8 +3277,11 @@
       <c r="R17" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S17" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -3202,8 +3314,11 @@
       <c r="R18" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S18" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>18</v>
       </c>
@@ -3238,8 +3353,11 @@
       <c r="R19" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S19" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -3272,8 +3390,11 @@
       <c r="R20" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S20" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -3306,8 +3427,11 @@
       <c r="R21" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S21" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -3342,8 +3466,11 @@
       <c r="R22" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S22" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -3376,8 +3503,11 @@
       <c r="R23" s="18">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S23" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -3410,8 +3540,11 @@
       <c r="R24" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S24" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>24</v>
       </c>
@@ -3444,8 +3577,11 @@
       <c r="R25" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S25" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>25</v>
       </c>
@@ -3478,8 +3614,11 @@
       <c r="R26" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S26" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>26</v>
       </c>
@@ -3514,8 +3653,11 @@
       <c r="R27" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S27" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>27</v>
       </c>
@@ -3550,8 +3692,11 @@
       <c r="R28" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S28" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>28</v>
       </c>
@@ -3584,8 +3729,11 @@
       <c r="R29" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S29" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>29</v>
       </c>
@@ -3620,8 +3768,11 @@
       <c r="R30" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S30" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <v>30</v>
       </c>
@@ -3658,9 +3809,11 @@
       <c r="R31" s="18">
         <v>2</v>
       </c>
-      <c r="S31" s="1"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S31" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <v>31</v>
       </c>
@@ -3693,8 +3846,11 @@
       <c r="R32" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S32" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>32</v>
       </c>
@@ -3727,8 +3883,11 @@
       <c r="R33" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S33" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>33</v>
       </c>
@@ -3761,8 +3920,11 @@
       <c r="R34" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S34" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>34</v>
       </c>
@@ -3799,8 +3961,11 @@
       <c r="R35" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S35" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>35</v>
       </c>
@@ -3835,8 +4000,11 @@
       <c r="R36" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S36" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
         <v>36</v>
       </c>
@@ -3871,8 +4039,11 @@
       <c r="R37" s="18">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S37" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>37</v>
       </c>
@@ -3905,8 +4076,11 @@
       <c r="R38" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S38" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="18">
         <v>38</v>
       </c>
@@ -3939,8 +4113,11 @@
       <c r="R39" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S39" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>39</v>
       </c>
@@ -3975,8 +4152,11 @@
       <c r="R40" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S40" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>40</v>
       </c>
@@ -4009,8 +4189,11 @@
       <c r="R41" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S41" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <v>41</v>
       </c>
@@ -4043,8 +4226,11 @@
       <c r="R42" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S42" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>42</v>
       </c>
@@ -4077,8 +4263,11 @@
       <c r="R43" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S43" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <v>43</v>
       </c>
@@ -4115,8 +4304,11 @@
       <c r="R44" s="18">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S44" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>44</v>
       </c>
@@ -4151,8 +4343,11 @@
       <c r="R45" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S45" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>45</v>
       </c>
@@ -4185,8 +4380,11 @@
       <c r="R46" s="18">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S46" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>46</v>
       </c>
@@ -4219,8 +4417,11 @@
       <c r="R47" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S47" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>47</v>
       </c>
@@ -4253,8 +4454,11 @@
       <c r="R48" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S48" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>48</v>
       </c>
@@ -4287,8 +4491,11 @@
       <c r="R49" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S49" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>49</v>
       </c>
@@ -4323,8 +4530,11 @@
       <c r="R50" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S50" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>50</v>
       </c>
@@ -4359,8 +4569,11 @@
       <c r="R51" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S51" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
         <v>51</v>
       </c>
@@ -4393,8 +4606,11 @@
       <c r="R52" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S52" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
         <v>52</v>
       </c>
@@ -4427,8 +4643,11 @@
       <c r="R53" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S53" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
         <v>53</v>
       </c>
@@ -4461,8 +4680,11 @@
       <c r="R54" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S54" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="18">
         <v>54</v>
       </c>
@@ -4495,8 +4717,11 @@
       <c r="R55" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S55" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
         <v>55</v>
       </c>
@@ -4529,8 +4754,11 @@
       <c r="R56" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S56" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
         <v>56</v>
       </c>
@@ -4563,8 +4791,11 @@
       <c r="R57" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S57" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <v>57</v>
       </c>
@@ -4599,8 +4830,11 @@
       <c r="R58" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S58" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <v>58</v>
       </c>
@@ -4633,8 +4867,11 @@
       <c r="R59" s="18">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S59" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <v>59</v>
       </c>
@@ -4667,9 +4904,11 @@
       <c r="R60" s="18">
         <v>5</v>
       </c>
-      <c r="S60" s="3"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S60" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <v>60</v>
       </c>
@@ -4702,8 +4941,11 @@
       <c r="R61" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S61" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <v>61</v>
       </c>
@@ -4736,8 +4978,11 @@
       <c r="R62" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S62" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
         <v>62</v>
       </c>
@@ -4770,8 +5015,11 @@
       <c r="R63" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S63" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
         <v>63</v>
       </c>
@@ -4806,8 +5054,11 @@
       <c r="R64" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S64" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="18">
         <v>64</v>
       </c>
@@ -4844,8 +5095,11 @@
       <c r="R65" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S65" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="18">
         <v>65</v>
       </c>
@@ -4880,8 +5134,11 @@
       <c r="R66" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S66" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="18">
         <v>66</v>
       </c>
@@ -4916,8 +5173,11 @@
       <c r="R67" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S67" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="18">
         <v>67</v>
       </c>
@@ -4950,8 +5210,11 @@
       <c r="R68" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S68" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="18">
         <v>68</v>
       </c>
@@ -4984,8 +5247,11 @@
       <c r="R69" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S69" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="18">
         <v>69</v>
       </c>
@@ -5018,8 +5284,11 @@
       <c r="R70" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S70" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
         <v>70</v>
       </c>
@@ -5052,8 +5321,11 @@
       <c r="R71" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S71" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
         <v>71</v>
       </c>
@@ -5086,8 +5358,11 @@
       <c r="R72" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S72" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="18">
         <v>72</v>
       </c>
@@ -5124,8 +5399,11 @@
       <c r="R73" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S73" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="18">
         <v>73</v>
       </c>
@@ -5158,8 +5436,11 @@
       <c r="R74" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S74" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="18">
         <v>74</v>
       </c>
@@ -5192,8 +5473,11 @@
       <c r="R75" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S75" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="18">
         <v>75</v>
       </c>
@@ -5228,8 +5512,11 @@
       <c r="R76" s="18">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S76" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18">
         <v>76</v>
       </c>
@@ -5264,8 +5551,11 @@
       <c r="R77" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S77" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
         <v>77</v>
       </c>
@@ -5300,8 +5590,11 @@
       <c r="R78" s="18">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S78" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
         <v>78</v>
       </c>
@@ -5334,8 +5627,11 @@
       <c r="R79" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S79" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
         <v>79</v>
       </c>
@@ -5370,8 +5666,11 @@
       <c r="R80" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S80" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="18">
         <v>80</v>
       </c>
@@ -5406,8 +5705,11 @@
       <c r="R81" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S81" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
         <v>81</v>
       </c>
@@ -5442,8 +5744,11 @@
       <c r="R82" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S82" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="18">
         <v>82</v>
       </c>
@@ -5476,8 +5781,11 @@
       <c r="R83" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S83" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="18">
         <v>83</v>
       </c>
@@ -5510,8 +5818,11 @@
       <c r="R84" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S84" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="18">
         <v>84</v>
       </c>
@@ -5544,8 +5855,11 @@
       <c r="R85" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S85" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="18">
         <v>85</v>
       </c>
@@ -5578,8 +5892,11 @@
       <c r="R86" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S86" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="18">
         <v>86</v>
       </c>
@@ -5616,8 +5933,11 @@
       <c r="R87" s="18">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S87" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="18">
         <v>87</v>
       </c>
@@ -5650,8 +5970,11 @@
       <c r="R88" s="18">
         <v>11</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S88" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="18">
         <v>88</v>
       </c>
@@ -5684,8 +6007,11 @@
       <c r="R89" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S89" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="18">
         <v>89</v>
       </c>
@@ -5720,8 +6046,11 @@
       <c r="R90" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S90" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="18">
         <v>90</v>
       </c>
@@ -5754,8 +6083,11 @@
       <c r="R91" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S91" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="18">
         <v>91</v>
       </c>
@@ -5788,8 +6120,11 @@
       <c r="R92" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S92" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="18">
         <v>92</v>
       </c>
@@ -5824,8 +6159,11 @@
       <c r="R93" s="18">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S93" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="18">
         <v>93</v>
       </c>
@@ -5858,8 +6196,11 @@
       <c r="R94" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S94" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="18">
         <v>94</v>
       </c>
@@ -5896,8 +6237,11 @@
       <c r="R95" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S95" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="18">
         <v>95</v>
       </c>
@@ -5930,8 +6274,11 @@
       <c r="R96" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S96" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="18">
         <v>96</v>
       </c>
@@ -5966,8 +6313,11 @@
       <c r="R97" s="18">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S97" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="18">
         <v>97</v>
       </c>
@@ -6004,8 +6354,11 @@
       <c r="R98" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S98" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="18">
         <v>98</v>
       </c>
@@ -6040,8 +6393,11 @@
       <c r="R99" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S99" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="18">
         <v>99</v>
       </c>
@@ -6074,8 +6430,11 @@
       <c r="R100" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S100" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="18">
         <v>100</v>
       </c>
@@ -6108,8 +6467,11 @@
       <c r="R101" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S101" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="18">
         <v>101</v>
       </c>
@@ -6142,8 +6504,11 @@
       <c r="R102" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S102" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="18">
         <v>102</v>
       </c>
@@ -6176,8 +6541,11 @@
       <c r="R103" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S103" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -6209,21 +6577,21 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" customWidth="1"/>
-    <col min="4" max="4" width="3.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G2" s="1" t="s">
         <v>42</v>
       </c>
@@ -6231,7 +6599,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G3" s="1">
         <v>17644936.100000001</v>
       </c>
@@ -6239,7 +6607,7 @@
         <v>204301.34</v>
       </c>
     </row>
-    <row r="4" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G4" s="1">
         <v>-166123.07999999999</v>
       </c>
@@ -6247,7 +6615,7 @@
         <v>98414.79</v>
       </c>
     </row>
-    <row r="5" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G5" s="1">
         <v>4900152.0999999996</v>
       </c>
@@ -6255,7 +6623,7 @@
         <v>3557905.85</v>
       </c>
     </row>
-    <row r="6" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G6" s="1">
         <v>286245</v>
       </c>
@@ -6263,7 +6631,7 @@
         <v>866744.93</v>
       </c>
     </row>
-    <row r="7" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G7" s="1">
         <v>619378.32999999996</v>
       </c>
@@ -6271,7 +6639,7 @@
         <v>161285.35999999999</v>
       </c>
     </row>
-    <row r="8" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G8" s="5">
         <f>SUM(G3:G7)</f>
         <v>23284588.450000003</v>
@@ -6280,7 +6648,7 @@
         <v>15775.98</v>
       </c>
     </row>
-    <row r="9" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G9" s="5">
         <v>28737182.920000002</v>
       </c>
@@ -6288,7 +6656,7 @@
         <v>14288.02</v>
       </c>
     </row>
-    <row r="10" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
       <c r="G10" s="5">
         <f>G9-G8</f>
         <v>5452594.4699999988</v>
@@ -6297,13 +6665,13 @@
         <v>53423.24</v>
       </c>
     </row>
-    <row r="11" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I11" s="5">
         <f>SUM(I3:I10)</f>
         <v>4972139.5100000007</v>
       </c>
     </row>
-    <row r="14" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
@@ -6311,7 +6679,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
         <v>875966.73300000001</v>
       </c>
@@ -6319,7 +6687,7 @@
         <v>46900.13</v>
       </c>
     </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
         <v>906433.66399999999</v>
       </c>
@@ -6327,7 +6695,7 @@
         <v>2590080.1800000002</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
         <f>SUM(E15:E16)</f>
         <v>1782400.3969999999</v>
@@ -6336,7 +6704,7 @@
         <v>1949709.13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
         <v>7172327.3300000001</v>
       </c>
@@ -6344,7 +6712,7 @@
         <v>1366206.83</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E19" s="5">
         <f>E18-E17</f>
         <v>5389926.9330000002</v>
@@ -6353,23 +6721,23 @@
         <v>739134.85</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G20" s="1">
         <v>379009.28000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G21" s="1">
         <v>600581.69999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G22" s="1">
         <f>SUM(G15:G21)</f>
         <v>7671622.0999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>77</v>
       </c>
@@ -6410,16 +6778,16 @@
       <selection activeCell="A2" sqref="A2:N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>75</v>
       </c>
@@ -6447,7 +6815,7 @@
         <v>4232587</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>76</v>
       </c>
@@ -6471,7 +6839,7 @@
         <v>8992806</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>77</v>
       </c>
@@ -6499,7 +6867,7 @@
         <v>5502837.0250000004</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>78</v>
       </c>
@@ -6527,7 +6895,7 @@
         <v>3191592</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
@@ -6553,7 +6921,7 @@
         <v>6275786</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>80</v>
       </c>
@@ -6577,7 +6945,7 @@
         <v>3061893</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>81</v>
       </c>
@@ -6601,7 +6969,7 @@
         <v>18223550</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>82</v>
       </c>
@@ -6625,7 +6993,7 @@
         <v>3211140</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>83</v>
       </c>
@@ -6658,18 +7026,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="21" width="9.77734375" customWidth="1"/>
-    <col min="22" max="22" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="21" width="9.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>244</v>
       </c>
@@ -6737,7 +7105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>265</v>
       </c>
@@ -6763,7 +7131,7 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>266</v>
       </c>
@@ -6789,7 +7157,7 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>267</v>
       </c>
@@ -6815,7 +7183,7 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>268</v>
       </c>
@@ -6841,7 +7209,7 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>143</v>
       </c>
@@ -6867,7 +7235,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>174</v>
       </c>
@@ -6893,7 +7261,7 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>269</v>
       </c>
@@ -6919,7 +7287,7 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>270</v>
       </c>
@@ -6945,7 +7313,7 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>271</v>
       </c>
@@ -6971,7 +7339,7 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>272</v>
       </c>
@@ -6997,7 +7365,7 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>131</v>
       </c>
@@ -7023,7 +7391,7 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>273</v>
       </c>
@@ -7049,7 +7417,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>274</v>
       </c>
@@ -7075,7 +7443,7 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>275</v>
       </c>
@@ -7101,7 +7469,7 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>276</v>
       </c>
@@ -7127,7 +7495,7 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>215</v>
       </c>
@@ -7153,7 +7521,7 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>277</v>
       </c>
@@ -7179,7 +7547,7 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>278</v>
       </c>
@@ -7205,7 +7573,7 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>279</v>
       </c>
@@ -7231,7 +7599,7 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>280</v>
       </c>
@@ -7257,7 +7625,7 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>110</v>
       </c>
@@ -7283,7 +7651,7 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>148</v>
       </c>
@@ -7309,7 +7677,7 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>281</v>
       </c>
@@ -7335,7 +7703,7 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>282</v>
       </c>
@@ -7361,7 +7729,7 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>283</v>
       </c>
@@ -7387,7 +7755,7 @@
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>284</v>
       </c>
@@ -7413,7 +7781,7 @@
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>300</v>
       </c>
@@ -7439,7 +7807,7 @@
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>301</v>
       </c>
@@ -7465,7 +7833,7 @@
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>302</v>
       </c>
@@ -7491,7 +7859,7 @@
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>129</v>
       </c>
@@ -7517,7 +7885,7 @@
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>205</v>
       </c>
@@ -7543,7 +7911,7 @@
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>162</v>
       </c>
@@ -7569,7 +7937,7 @@
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>196</v>
       </c>
@@ -7595,7 +7963,7 @@
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>181</v>
       </c>
@@ -7621,7 +7989,7 @@
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>203</v>
       </c>
@@ -7647,7 +8015,7 @@
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>285</v>
       </c>
@@ -7673,7 +8041,7 @@
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>286</v>
       </c>
@@ -7699,7 +8067,7 @@
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>287</v>
       </c>
@@ -7725,7 +8093,7 @@
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>288</v>
       </c>
@@ -7751,7 +8119,7 @@
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>289</v>
       </c>
@@ -7777,7 +8145,7 @@
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>290</v>
       </c>
@@ -7803,7 +8171,7 @@
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>291</v>
       </c>
@@ -7829,7 +8197,7 @@
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>292</v>
       </c>
@@ -7855,7 +8223,7 @@
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>293</v>
       </c>
@@ -7881,7 +8249,7 @@
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>169</v>
       </c>
@@ -7907,7 +8275,7 @@
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>125</v>
       </c>
@@ -7933,7 +8301,7 @@
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>149</v>
       </c>
@@ -7959,7 +8327,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>294</v>
       </c>
@@ -7985,7 +8353,7 @@
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>295</v>
       </c>
@@ -8011,7 +8379,7 @@
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>146</v>
       </c>
@@ -8037,7 +8405,7 @@
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>296</v>
       </c>
@@ -8063,7 +8431,7 @@
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>93</v>
       </c>
@@ -8089,7 +8457,7 @@
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
         <v>95</v>
       </c>
@@ -8115,7 +8483,7 @@
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>297</v>
       </c>
@@ -8144,4 +8512,628 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="13" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+    </row>
+    <row r="15" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+    </row>
+    <row r="16" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+    </row>
+    <row r="17" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+    </row>
+    <row r="18" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+    </row>
+    <row r="19" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+    </row>
+    <row r="20" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+    </row>
+    <row r="21" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+    </row>
+    <row r="22" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+    </row>
+    <row r="23" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+    </row>
+    <row r="24" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+    </row>
+    <row r="25" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+    </row>
+    <row r="26" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+    </row>
+    <row r="27" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+    </row>
+    <row r="28" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
+    </row>
+    <row r="29" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
+      <c r="C29" s="34"/>
+    </row>
+    <row r="30" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
+    </row>
+    <row r="31" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
+    </row>
+    <row r="32" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+    </row>
+    <row r="33" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+    </row>
+    <row r="34" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+    </row>
+    <row r="35" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+    </row>
+    <row r="36" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+    </row>
+    <row r="37" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
+    </row>
+    <row r="38" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
+    </row>
+    <row r="39" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="32"/>
+    </row>
+    <row r="40" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="32"/>
+    </row>
+    <row r="41" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32"/>
+    </row>
+    <row r="42" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32"/>
+    </row>
+    <row r="43" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32"/>
+    </row>
+    <row r="44" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32"/>
+    </row>
+    <row r="45" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
+    </row>
+    <row r="46" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32"/>
+    </row>
+    <row r="47" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32"/>
+    </row>
+    <row r="48" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
+    </row>
+    <row r="49" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
+    </row>
+    <row r="50" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="32"/>
+    </row>
+    <row r="51" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
+    </row>
+    <row r="52" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="32"/>
+    </row>
+    <row r="53" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="35"/>
+    </row>
+    <row r="54" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
+    </row>
+    <row r="55" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="13" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>